<commit_message>
Added file cleaning feature
</commit_message>
<xml_diff>
--- a/data_for_bsh/DataEntries.xlsx
+++ b/data_for_bsh/DataEntries.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
   <si>
     <t>  ConferencePublication</t>
   </si>
@@ -138,7 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +168,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +196,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -246,13 +258,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -263,11 +276,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -549,7 +564,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,14 +744,14 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -882,7 +897,9 @@
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="C24" s="5" t="s">
         <v>29</v>
       </c>

</xml_diff>